<commit_message>
working on logs for errors handling, partly finished
</commit_message>
<xml_diff>
--- a/Registration files/Service_list.xlsx
+++ b/Registration files/Service_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,39 +589,223 @@
       <c r="C4" t="n">
         <v>992907510905</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>1.234567891234568e+16</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Toyota Camry 6</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Service 4</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>30/08/2025</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-08-09 12:03:57</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>No comments</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>8138074349</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Yo yo</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>992907510905</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.234567891234568e+16</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Camry 10</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Service 3</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>13/08/2025</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-08-11 09:30:28</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8138074349</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Yo yo</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>992907510905</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.235467891234568e+16</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Service 1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>16/08/2025</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-08-11 09:35:39</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>8138074349</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Yo yo</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>992907510905</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.234567891234568e+16</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Toyota Camry 6</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Service 2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>13/08/2025</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-08-11 10:47:28</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8138074349</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Yo yo</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>992907510905</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>12345678912345678</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Toyota Camry 6</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Service 4</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Service 3</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>30/08/2025</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2025-08-09 12:03:57</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>No comments</t>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-08-11 12:03:40</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nope</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Made language for test drive and service
</commit_message>
<xml_diff>
--- a/Registration files/Service_list.xlsx
+++ b/Registration files/Service_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,10 +635,8 @@
       <c r="C5" t="n">
         <v>992938636344</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>12345678901234567</t>
-        </is>
+      <c r="D5" t="n">
+        <v>1.234567890123457e+16</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -666,6 +664,100 @@
         </is>
       </c>
       <c r="J5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>631886740</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ikki maru</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>992907510905</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.234567891234568e+16</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Toyota Camry MILLION</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Регулярное обслуживание</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-08-22 14:44:41</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>631886740</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ikki maru</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>992907510905</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>12345678912345678</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Toyota Land Cruiser</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Регулярное обслуживание</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>23/08/2025</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-08-22 16:50:58</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
sent few photos/broadcast check
</commit_message>
<xml_diff>
--- a/Registration files/Service_list.xlsx
+++ b/Registration files/Service_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,10 +727,8 @@
       <c r="C7" t="n">
         <v>992907510905</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>12345678912345678</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1.234567891234568e+16</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -758,6 +756,54 @@
         </is>
       </c>
       <c r="J7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5547528084</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Хушдил Саидов</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>79177131361</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12344455566677788</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TOYOTA COROLLA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Осмотр</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>27/08/2025</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-08-26 08:47:50</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>